<commit_message>
Update tags to align with lang-otw #1
</commit_message>
<xml_diff>
--- a/createYaml/VII.xlsx
+++ b/createYaml/VII.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/Desktop/createYaml/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/Desktop/Current-Projects/ParserTools/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96857EFD-1F49-184A-8723-91A625F7A841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0E53E6-B686-1446-BB22-97C9645361BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="760" windowWidth="23340" windowHeight="20460" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
+    <workbookView xWindow="-27320" yWindow="4080" windowWidth="23340" windowHeight="14860" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
   <sheets>
     <sheet name="VII_IND" sheetId="1" r:id="rId1"/>
@@ -1062,9 +1062,6 @@
     <t>VII</t>
   </si>
   <si>
-    <t>Conjunct</t>
-  </si>
-  <si>
     <t>Lexeme</t>
   </si>
   <si>
@@ -1092,7 +1089,10 @@
     <t>atemagasininiibanen</t>
   </si>
   <si>
-    <t>Independent</t>
+    <t>Ind</t>
+  </si>
+  <si>
+    <t>Cnj</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA193F61-3C0D-9941-81CC-6F6AD6C92B40}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1476,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1499,7 +1499,7 @@
         <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1525,7 +1525,7 @@
         <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1551,7 +1551,7 @@
         <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1577,7 +1577,7 @@
         <v>341</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1603,7 +1603,7 @@
         <v>341</v>
       </c>
       <c r="B6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1629,7 +1629,7 @@
         <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1655,7 +1655,7 @@
         <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1681,7 +1681,7 @@
         <v>341</v>
       </c>
       <c r="B9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1707,7 +1707,7 @@
         <v>341</v>
       </c>
       <c r="B10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1733,7 +1733,7 @@
         <v>341</v>
       </c>
       <c r="B11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1762,7 +1762,7 @@
         <v>341</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1788,7 +1788,7 @@
         <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1817,7 +1817,7 @@
         <v>341</v>
       </c>
       <c r="B14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -1843,7 +1843,7 @@
         <v>341</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1872,7 +1872,7 @@
         <v>341</v>
       </c>
       <c r="B16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -1898,7 +1898,7 @@
         <v>341</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1927,7 +1927,7 @@
         <v>341</v>
       </c>
       <c r="B18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -1953,7 +1953,7 @@
         <v>341</v>
       </c>
       <c r="B19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1979,7 +1979,7 @@
         <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -2005,7 +2005,7 @@
         <v>341</v>
       </c>
       <c r="B21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -2031,7 +2031,7 @@
         <v>341</v>
       </c>
       <c r="B22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -2057,7 +2057,7 @@
         <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -2083,7 +2083,7 @@
         <v>341</v>
       </c>
       <c r="B24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -2109,7 +2109,7 @@
         <v>341</v>
       </c>
       <c r="B25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -2135,7 +2135,7 @@
         <v>341</v>
       </c>
       <c r="B26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -2161,7 +2161,7 @@
         <v>341</v>
       </c>
       <c r="B27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -2190,7 +2190,7 @@
         <v>341</v>
       </c>
       <c r="B28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -2216,7 +2216,7 @@
         <v>341</v>
       </c>
       <c r="B29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -2245,7 +2245,7 @@
         <v>341</v>
       </c>
       <c r="B30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -2271,7 +2271,7 @@
         <v>341</v>
       </c>
       <c r="B31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -2300,7 +2300,7 @@
         <v>341</v>
       </c>
       <c r="B32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -2326,7 +2326,7 @@
         <v>341</v>
       </c>
       <c r="B33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -2355,7 +2355,7 @@
         <v>341</v>
       </c>
       <c r="B34" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
@@ -2381,7 +2381,7 @@
         <v>341</v>
       </c>
       <c r="B35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
@@ -2407,7 +2407,7 @@
         <v>341</v>
       </c>
       <c r="B36" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -2433,7 +2433,7 @@
         <v>341</v>
       </c>
       <c r="B37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
@@ -2459,7 +2459,7 @@
         <v>341</v>
       </c>
       <c r="B38" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -2485,7 +2485,7 @@
         <v>341</v>
       </c>
       <c r="B39" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
@@ -2511,7 +2511,7 @@
         <v>341</v>
       </c>
       <c r="B40" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
@@ -2537,7 +2537,7 @@
         <v>341</v>
       </c>
       <c r="B41" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -2563,7 +2563,7 @@
         <v>341</v>
       </c>
       <c r="B42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -2589,7 +2589,7 @@
         <v>341</v>
       </c>
       <c r="B43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -2618,7 +2618,7 @@
         <v>341</v>
       </c>
       <c r="B44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -2644,7 +2644,7 @@
         <v>341</v>
       </c>
       <c r="B45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -2673,7 +2673,7 @@
         <v>341</v>
       </c>
       <c r="B46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
@@ -2699,7 +2699,7 @@
         <v>341</v>
       </c>
       <c r="B47" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
@@ -2728,7 +2728,7 @@
         <v>341</v>
       </c>
       <c r="B48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -2754,7 +2754,7 @@
         <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
@@ -2775,7 +2775,7 @@
         <v>127</v>
       </c>
       <c r="I49" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2783,7 +2783,7 @@
         <v>341</v>
       </c>
       <c r="B50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C50" t="s">
         <v>23</v>
@@ -2809,7 +2809,7 @@
         <v>341</v>
       </c>
       <c r="B51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
@@ -2835,7 +2835,7 @@
         <v>341</v>
       </c>
       <c r="B52" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C52" t="s">
         <v>23</v>
@@ -2861,7 +2861,7 @@
         <v>341</v>
       </c>
       <c r="B53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
@@ -2887,7 +2887,7 @@
         <v>341</v>
       </c>
       <c r="B54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -2913,7 +2913,7 @@
         <v>341</v>
       </c>
       <c r="B55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -2939,7 +2939,7 @@
         <v>341</v>
       </c>
       <c r="B56" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C56" t="s">
         <v>23</v>
@@ -2965,7 +2965,7 @@
         <v>341</v>
       </c>
       <c r="B57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C57" t="s">
         <v>23</v>
@@ -2991,7 +2991,7 @@
         <v>341</v>
       </c>
       <c r="B58" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C58" t="s">
         <v>23</v>
@@ -3017,7 +3017,7 @@
         <v>341</v>
       </c>
       <c r="B59" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C59" t="s">
         <v>23</v>
@@ -3046,7 +3046,7 @@
         <v>341</v>
       </c>
       <c r="B60" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C60" t="s">
         <v>23</v>
@@ -3072,7 +3072,7 @@
         <v>341</v>
       </c>
       <c r="B61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
@@ -3101,7 +3101,7 @@
         <v>341</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
@@ -3127,7 +3127,7 @@
         <v>341</v>
       </c>
       <c r="B63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C63" t="s">
         <v>23</v>
@@ -3156,7 +3156,7 @@
         <v>341</v>
       </c>
       <c r="B64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C64" t="s">
         <v>23</v>
@@ -3182,7 +3182,7 @@
         <v>341</v>
       </c>
       <c r="B65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C65" t="s">
         <v>23</v>
@@ -3211,7 +3211,7 @@
         <v>341</v>
       </c>
       <c r="B66" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C66" t="s">
         <v>13</v>
@@ -3237,7 +3237,7 @@
         <v>341</v>
       </c>
       <c r="B67" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C67" t="s">
         <v>13</v>
@@ -3263,7 +3263,7 @@
         <v>341</v>
       </c>
       <c r="B68" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C68" t="s">
         <v>13</v>
@@ -3289,7 +3289,7 @@
         <v>341</v>
       </c>
       <c r="B69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C69" t="s">
         <v>13</v>
@@ -3315,7 +3315,7 @@
         <v>341</v>
       </c>
       <c r="B70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C70" t="s">
         <v>13</v>
@@ -3341,7 +3341,7 @@
         <v>341</v>
       </c>
       <c r="B71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C71" t="s">
         <v>13</v>
@@ -3367,7 +3367,7 @@
         <v>341</v>
       </c>
       <c r="B72" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C72" t="s">
         <v>13</v>
@@ -3393,7 +3393,7 @@
         <v>341</v>
       </c>
       <c r="B73" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C73" t="s">
         <v>13</v>
@@ -3419,7 +3419,7 @@
         <v>341</v>
       </c>
       <c r="B74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C74" t="s">
         <v>13</v>
@@ -3445,7 +3445,7 @@
         <v>341</v>
       </c>
       <c r="B75" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C75" t="s">
         <v>13</v>
@@ -3474,7 +3474,7 @@
         <v>341</v>
       </c>
       <c r="B76" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C76" t="s">
         <v>13</v>
@@ -3500,7 +3500,7 @@
         <v>341</v>
       </c>
       <c r="B77" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C77" t="s">
         <v>13</v>
@@ -3529,7 +3529,7 @@
         <v>341</v>
       </c>
       <c r="B78" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
@@ -3555,7 +3555,7 @@
         <v>341</v>
       </c>
       <c r="B79" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
@@ -3584,7 +3584,7 @@
         <v>341</v>
       </c>
       <c r="B80" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C80" t="s">
         <v>13</v>
@@ -3610,7 +3610,7 @@
         <v>341</v>
       </c>
       <c r="B81" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C81" t="s">
         <v>13</v>
@@ -3639,7 +3639,7 @@
         <v>341</v>
       </c>
       <c r="B82" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C82" t="s">
         <v>13</v>
@@ -3665,7 +3665,7 @@
         <v>341</v>
       </c>
       <c r="B83" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
@@ -3683,7 +3683,7 @@
         <v>8</v>
       </c>
       <c r="H83" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -3691,7 +3691,7 @@
         <v>341</v>
       </c>
       <c r="B84" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C84" t="s">
         <v>13</v>
@@ -3717,7 +3717,7 @@
         <v>341</v>
       </c>
       <c r="B85" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C85" t="s">
         <v>13</v>
@@ -3743,7 +3743,7 @@
         <v>341</v>
       </c>
       <c r="B86" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C86" t="s">
         <v>13</v>
@@ -3769,7 +3769,7 @@
         <v>341</v>
       </c>
       <c r="B87" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C87" t="s">
         <v>13</v>
@@ -3795,7 +3795,7 @@
         <v>341</v>
       </c>
       <c r="B88" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C88" t="s">
         <v>13</v>
@@ -3821,7 +3821,7 @@
         <v>341</v>
       </c>
       <c r="B89" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C89" t="s">
         <v>13</v>
@@ -3847,7 +3847,7 @@
         <v>341</v>
       </c>
       <c r="B90" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C90" t="s">
         <v>13</v>
@@ -3873,7 +3873,7 @@
         <v>341</v>
       </c>
       <c r="B91" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C91" t="s">
         <v>13</v>
@@ -3902,7 +3902,7 @@
         <v>341</v>
       </c>
       <c r="B92" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C92" t="s">
         <v>13</v>
@@ -3928,7 +3928,7 @@
         <v>341</v>
       </c>
       <c r="B93" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C93" t="s">
         <v>13</v>
@@ -3957,7 +3957,7 @@
         <v>341</v>
       </c>
       <c r="B94" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C94" t="s">
         <v>13</v>
@@ -3983,7 +3983,7 @@
         <v>341</v>
       </c>
       <c r="B95" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C95" t="s">
         <v>13</v>
@@ -4012,7 +4012,7 @@
         <v>341</v>
       </c>
       <c r="B96" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C96" t="s">
         <v>13</v>
@@ -4038,7 +4038,7 @@
         <v>341</v>
       </c>
       <c r="B97" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C97" t="s">
         <v>13</v>
@@ -4067,13 +4067,13 @@
         <v>341</v>
       </c>
       <c r="B98" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C98" t="s">
         <v>37</v>
       </c>
       <c r="D98" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E98" t="s">
         <v>335</v>
@@ -4093,13 +4093,13 @@
         <v>341</v>
       </c>
       <c r="B99" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C99" t="s">
         <v>37</v>
       </c>
       <c r="D99" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E99" t="s">
         <v>336</v>
@@ -4116,13 +4116,13 @@
         <v>341</v>
       </c>
       <c r="B100" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C100" t="s">
         <v>37</v>
       </c>
       <c r="D100" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E100" t="s">
         <v>337</v>
@@ -4142,13 +4142,13 @@
         <v>341</v>
       </c>
       <c r="B101" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C101" t="s">
         <v>37</v>
       </c>
       <c r="D101" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E101" t="s">
         <v>338</v>
@@ -4165,13 +4165,13 @@
         <v>341</v>
       </c>
       <c r="B102" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C102" t="s">
         <v>37</v>
       </c>
       <c r="D102" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E102" t="s">
         <v>335</v>
@@ -4191,13 +4191,13 @@
         <v>341</v>
       </c>
       <c r="B103" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C103" t="s">
         <v>37</v>
       </c>
       <c r="D103" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E103" t="s">
         <v>336</v>
@@ -4214,13 +4214,13 @@
         <v>341</v>
       </c>
       <c r="B104" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C104" t="s">
         <v>37</v>
       </c>
       <c r="D104" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E104" t="s">
         <v>337</v>
@@ -4240,13 +4240,13 @@
         <v>341</v>
       </c>
       <c r="B105" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C105" t="s">
         <v>37</v>
       </c>
       <c r="D105" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E105" t="s">
         <v>338</v>
@@ -4263,13 +4263,13 @@
         <v>341</v>
       </c>
       <c r="B106" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C106" t="s">
         <v>37</v>
       </c>
       <c r="D106" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E106" t="s">
         <v>335</v>
@@ -4286,13 +4286,13 @@
         <v>341</v>
       </c>
       <c r="B107" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C107" t="s">
         <v>37</v>
       </c>
       <c r="D107" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E107" t="s">
         <v>336</v>
@@ -4309,13 +4309,13 @@
         <v>341</v>
       </c>
       <c r="B108" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C108" t="s">
         <v>37</v>
       </c>
       <c r="D108" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E108" t="s">
         <v>337</v>
@@ -4332,13 +4332,13 @@
         <v>341</v>
       </c>
       <c r="B109" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C109" t="s">
         <v>37</v>
       </c>
       <c r="D109" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E109" t="s">
         <v>338</v>
@@ -4355,13 +4355,13 @@
         <v>341</v>
       </c>
       <c r="B110" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C110" t="s">
         <v>37</v>
       </c>
       <c r="D110" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E110" t="s">
         <v>335</v>
@@ -4378,13 +4378,13 @@
         <v>341</v>
       </c>
       <c r="B111" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C111" t="s">
         <v>37</v>
       </c>
       <c r="D111" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E111" t="s">
         <v>336</v>
@@ -4401,13 +4401,13 @@
         <v>341</v>
       </c>
       <c r="B112" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C112" t="s">
         <v>37</v>
       </c>
       <c r="D112" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E112" t="s">
         <v>337</v>
@@ -4424,13 +4424,13 @@
         <v>341</v>
       </c>
       <c r="B113" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C113" t="s">
         <v>37</v>
       </c>
       <c r="D113" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E113" t="s">
         <v>338</v>
@@ -4447,13 +4447,13 @@
         <v>341</v>
       </c>
       <c r="B114" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C114" t="s">
         <v>37</v>
       </c>
       <c r="D114" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E114" t="s">
         <v>335</v>
@@ -4470,13 +4470,13 @@
         <v>341</v>
       </c>
       <c r="B115" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C115" t="s">
         <v>37</v>
       </c>
       <c r="D115" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E115" t="s">
         <v>336</v>
@@ -4493,13 +4493,13 @@
         <v>341</v>
       </c>
       <c r="B116" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C116" t="s">
         <v>37</v>
       </c>
       <c r="D116" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E116" t="s">
         <v>337</v>
@@ -4516,13 +4516,13 @@
         <v>341</v>
       </c>
       <c r="B117" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C117" t="s">
         <v>37</v>
       </c>
       <c r="D117" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E117" t="s">
         <v>338</v>
@@ -4539,13 +4539,13 @@
         <v>341</v>
       </c>
       <c r="B118" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C118" t="s">
         <v>37</v>
       </c>
       <c r="D118" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E118" t="s">
         <v>335</v>
@@ -4562,13 +4562,13 @@
         <v>341</v>
       </c>
       <c r="B119" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C119" t="s">
         <v>37</v>
       </c>
       <c r="D119" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E119" t="s">
         <v>336</v>
@@ -4585,13 +4585,13 @@
         <v>341</v>
       </c>
       <c r="B120" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C120" t="s">
         <v>37</v>
       </c>
       <c r="D120" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E120" t="s">
         <v>337</v>
@@ -4608,13 +4608,13 @@
         <v>341</v>
       </c>
       <c r="B121" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C121" t="s">
         <v>37</v>
       </c>
       <c r="D121" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E121" t="s">
         <v>338</v>
@@ -4631,13 +4631,13 @@
         <v>341</v>
       </c>
       <c r="B122" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C122" t="s">
         <v>37</v>
       </c>
       <c r="D122" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E122" t="s">
         <v>335</v>
@@ -4654,13 +4654,13 @@
         <v>341</v>
       </c>
       <c r="B123" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C123" t="s">
         <v>37</v>
       </c>
       <c r="D123" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E123" t="s">
         <v>336</v>
@@ -4677,13 +4677,13 @@
         <v>341</v>
       </c>
       <c r="B124" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C124" t="s">
         <v>37</v>
       </c>
       <c r="D124" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E124" t="s">
         <v>337</v>
@@ -4700,13 +4700,13 @@
         <v>341</v>
       </c>
       <c r="B125" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C125" t="s">
         <v>37</v>
       </c>
       <c r="D125" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E125" t="s">
         <v>338</v>
@@ -4723,13 +4723,13 @@
         <v>341</v>
       </c>
       <c r="B126" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C126" t="s">
         <v>37</v>
       </c>
       <c r="D126" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E126" t="s">
         <v>335</v>
@@ -4746,13 +4746,13 @@
         <v>341</v>
       </c>
       <c r="B127" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C127" t="s">
         <v>37</v>
       </c>
       <c r="D127" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E127" t="s">
         <v>336</v>
@@ -4769,13 +4769,13 @@
         <v>341</v>
       </c>
       <c r="B128" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C128" t="s">
         <v>37</v>
       </c>
       <c r="D128" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E128" t="s">
         <v>337</v>
@@ -4792,13 +4792,13 @@
         <v>341</v>
       </c>
       <c r="B129" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C129" t="s">
         <v>37</v>
       </c>
       <c r="D129" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E129" t="s">
         <v>338</v>
@@ -4815,7 +4815,7 @@
         <v>341</v>
       </c>
       <c r="B130" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C130" t="s">
         <v>18</v>
@@ -4841,7 +4841,7 @@
         <v>341</v>
       </c>
       <c r="B131" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C131" t="s">
         <v>18</v>
@@ -4867,7 +4867,7 @@
         <v>341</v>
       </c>
       <c r="B132" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C132" t="s">
         <v>18</v>
@@ -4893,7 +4893,7 @@
         <v>341</v>
       </c>
       <c r="B133" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C133" t="s">
         <v>18</v>
@@ -4919,7 +4919,7 @@
         <v>341</v>
       </c>
       <c r="B134" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C134" t="s">
         <v>18</v>
@@ -4945,7 +4945,7 @@
         <v>341</v>
       </c>
       <c r="B135" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C135" t="s">
         <v>18</v>
@@ -4971,7 +4971,7 @@
         <v>341</v>
       </c>
       <c r="B136" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C136" t="s">
         <v>18</v>
@@ -4997,7 +4997,7 @@
         <v>341</v>
       </c>
       <c r="B137" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C137" t="s">
         <v>18</v>
@@ -5023,7 +5023,7 @@
         <v>341</v>
       </c>
       <c r="B138" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C138" t="s">
         <v>18</v>
@@ -5049,7 +5049,7 @@
         <v>341</v>
       </c>
       <c r="B139" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C139" t="s">
         <v>18</v>
@@ -5078,7 +5078,7 @@
         <v>341</v>
       </c>
       <c r="B140" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C140" t="s">
         <v>18</v>
@@ -5104,7 +5104,7 @@
         <v>341</v>
       </c>
       <c r="B141" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C141" t="s">
         <v>18</v>
@@ -5133,7 +5133,7 @@
         <v>341</v>
       </c>
       <c r="B142" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C142" t="s">
         <v>18</v>
@@ -5159,7 +5159,7 @@
         <v>341</v>
       </c>
       <c r="B143" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C143" t="s">
         <v>18</v>
@@ -5188,7 +5188,7 @@
         <v>341</v>
       </c>
       <c r="B144" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C144" t="s">
         <v>18</v>
@@ -5214,7 +5214,7 @@
         <v>341</v>
       </c>
       <c r="B145" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C145" t="s">
         <v>18</v>
@@ -5235,7 +5235,7 @@
         <v>122</v>
       </c>
       <c r="I145" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -5243,7 +5243,7 @@
         <v>341</v>
       </c>
       <c r="B146" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C146" t="s">
         <v>18</v>
@@ -5269,7 +5269,7 @@
         <v>341</v>
       </c>
       <c r="B147" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C147" t="s">
         <v>18</v>
@@ -5295,7 +5295,7 @@
         <v>341</v>
       </c>
       <c r="B148" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C148" t="s">
         <v>18</v>
@@ -5321,7 +5321,7 @@
         <v>341</v>
       </c>
       <c r="B149" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C149" t="s">
         <v>18</v>
@@ -5347,7 +5347,7 @@
         <v>341</v>
       </c>
       <c r="B150" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C150" t="s">
         <v>18</v>
@@ -5373,7 +5373,7 @@
         <v>341</v>
       </c>
       <c r="B151" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C151" t="s">
         <v>18</v>
@@ -5399,7 +5399,7 @@
         <v>341</v>
       </c>
       <c r="B152" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C152" t="s">
         <v>18</v>
@@ -5425,7 +5425,7 @@
         <v>341</v>
       </c>
       <c r="B153" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C153" t="s">
         <v>18</v>
@@ -5451,7 +5451,7 @@
         <v>341</v>
       </c>
       <c r="B154" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C154" t="s">
         <v>18</v>
@@ -5477,7 +5477,7 @@
         <v>341</v>
       </c>
       <c r="B155" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C155" t="s">
         <v>18</v>
@@ -5506,7 +5506,7 @@
         <v>341</v>
       </c>
       <c r="B156" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C156" t="s">
         <v>18</v>
@@ -5532,7 +5532,7 @@
         <v>341</v>
       </c>
       <c r="B157" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C157" t="s">
         <v>18</v>
@@ -5561,7 +5561,7 @@
         <v>341</v>
       </c>
       <c r="B158" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C158" t="s">
         <v>18</v>
@@ -5587,7 +5587,7 @@
         <v>341</v>
       </c>
       <c r="B159" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C159" t="s">
         <v>18</v>
@@ -5616,7 +5616,7 @@
         <v>341</v>
       </c>
       <c r="B160" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C160" t="s">
         <v>18</v>
@@ -5642,7 +5642,7 @@
         <v>341</v>
       </c>
       <c r="B161" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C161" t="s">
         <v>18</v>
@@ -5671,7 +5671,7 @@
         <v>341</v>
       </c>
       <c r="B162" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C162" t="s">
         <v>28</v>
@@ -5697,7 +5697,7 @@
         <v>341</v>
       </c>
       <c r="B163" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C163" t="s">
         <v>28</v>
@@ -5715,7 +5715,7 @@
         <v>8</v>
       </c>
       <c r="H163" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
@@ -5723,7 +5723,7 @@
         <v>341</v>
       </c>
       <c r="B164" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C164" t="s">
         <v>28</v>
@@ -5749,7 +5749,7 @@
         <v>341</v>
       </c>
       <c r="B165" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C165" t="s">
         <v>28</v>
@@ -5775,7 +5775,7 @@
         <v>341</v>
       </c>
       <c r="B166" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C166" t="s">
         <v>28</v>
@@ -5801,7 +5801,7 @@
         <v>341</v>
       </c>
       <c r="B167" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C167" t="s">
         <v>28</v>
@@ -5827,7 +5827,7 @@
         <v>341</v>
       </c>
       <c r="B168" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C168" t="s">
         <v>28</v>
@@ -5853,7 +5853,7 @@
         <v>341</v>
       </c>
       <c r="B169" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C169" t="s">
         <v>28</v>
@@ -5879,7 +5879,7 @@
         <v>341</v>
       </c>
       <c r="B170" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C170" t="s">
         <v>28</v>
@@ -5905,7 +5905,7 @@
         <v>341</v>
       </c>
       <c r="B171" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C171" t="s">
         <v>28</v>
@@ -5934,7 +5934,7 @@
         <v>341</v>
       </c>
       <c r="B172" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C172" t="s">
         <v>28</v>
@@ -5960,7 +5960,7 @@
         <v>341</v>
       </c>
       <c r="B173" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C173" t="s">
         <v>28</v>
@@ -5989,7 +5989,7 @@
         <v>341</v>
       </c>
       <c r="B174" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C174" t="s">
         <v>28</v>
@@ -6015,7 +6015,7 @@
         <v>341</v>
       </c>
       <c r="B175" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C175" t="s">
         <v>28</v>
@@ -6036,7 +6036,7 @@
         <v>129</v>
       </c>
       <c r="I175" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -6044,7 +6044,7 @@
         <v>341</v>
       </c>
       <c r="B176" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C176" t="s">
         <v>28</v>
@@ -6070,7 +6070,7 @@
         <v>341</v>
       </c>
       <c r="B177" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C177" t="s">
         <v>28</v>
@@ -6091,7 +6091,7 @@
         <v>131</v>
       </c>
       <c r="I177" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -6099,7 +6099,7 @@
         <v>341</v>
       </c>
       <c r="B178" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C178" t="s">
         <v>28</v>
@@ -6125,7 +6125,7 @@
         <v>341</v>
       </c>
       <c r="B179" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C179" t="s">
         <v>28</v>
@@ -6151,7 +6151,7 @@
         <v>341</v>
       </c>
       <c r="B180" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C180" t="s">
         <v>28</v>
@@ -6177,7 +6177,7 @@
         <v>341</v>
       </c>
       <c r="B181" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C181" t="s">
         <v>28</v>
@@ -6203,7 +6203,7 @@
         <v>341</v>
       </c>
       <c r="B182" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C182" t="s">
         <v>28</v>
@@ -6229,7 +6229,7 @@
         <v>341</v>
       </c>
       <c r="B183" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C183" t="s">
         <v>28</v>
@@ -6255,7 +6255,7 @@
         <v>341</v>
       </c>
       <c r="B184" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C184" t="s">
         <v>28</v>
@@ -6281,7 +6281,7 @@
         <v>341</v>
       </c>
       <c r="B185" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C185" t="s">
         <v>28</v>
@@ -6307,7 +6307,7 @@
         <v>341</v>
       </c>
       <c r="B186" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C186" t="s">
         <v>28</v>
@@ -6333,7 +6333,7 @@
         <v>341</v>
       </c>
       <c r="B187" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C187" t="s">
         <v>28</v>
@@ -6362,7 +6362,7 @@
         <v>341</v>
       </c>
       <c r="B188" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C188" t="s">
         <v>28</v>
@@ -6388,7 +6388,7 @@
         <v>341</v>
       </c>
       <c r="B189" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C189" t="s">
         <v>28</v>
@@ -6417,7 +6417,7 @@
         <v>341</v>
       </c>
       <c r="B190" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C190" t="s">
         <v>28</v>
@@ -6443,7 +6443,7 @@
         <v>341</v>
       </c>
       <c r="B191" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C191" t="s">
         <v>28</v>
@@ -6472,7 +6472,7 @@
         <v>341</v>
       </c>
       <c r="B192" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C192" t="s">
         <v>28</v>
@@ -6498,7 +6498,7 @@
         <v>341</v>
       </c>
       <c r="B193" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C193" t="s">
         <v>28</v>
@@ -6527,7 +6527,7 @@
         <v>341</v>
       </c>
       <c r="B194" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C194" t="s">
         <v>32</v>
@@ -6553,7 +6553,7 @@
         <v>341</v>
       </c>
       <c r="B195" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C195" t="s">
         <v>32</v>
@@ -6579,7 +6579,7 @@
         <v>341</v>
       </c>
       <c r="B196" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C196" t="s">
         <v>32</v>
@@ -6605,7 +6605,7 @@
         <v>341</v>
       </c>
       <c r="B197" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C197" t="s">
         <v>32</v>
@@ -6631,7 +6631,7 @@
         <v>341</v>
       </c>
       <c r="B198" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C198" t="s">
         <v>32</v>
@@ -6657,7 +6657,7 @@
         <v>341</v>
       </c>
       <c r="B199" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C199" t="s">
         <v>32</v>
@@ -6683,7 +6683,7 @@
         <v>341</v>
       </c>
       <c r="B200" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C200" t="s">
         <v>32</v>
@@ -6709,7 +6709,7 @@
         <v>341</v>
       </c>
       <c r="B201" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C201" t="s">
         <v>32</v>
@@ -6735,7 +6735,7 @@
         <v>341</v>
       </c>
       <c r="B202" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C202" t="s">
         <v>32</v>
@@ -6761,7 +6761,7 @@
         <v>341</v>
       </c>
       <c r="B203" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C203" t="s">
         <v>32</v>
@@ -6790,7 +6790,7 @@
         <v>341</v>
       </c>
       <c r="B204" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C204" t="s">
         <v>32</v>
@@ -6816,7 +6816,7 @@
         <v>341</v>
       </c>
       <c r="B205" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C205" t="s">
         <v>32</v>
@@ -6845,7 +6845,7 @@
         <v>341</v>
       </c>
       <c r="B206" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C206" t="s">
         <v>32</v>
@@ -6871,7 +6871,7 @@
         <v>341</v>
       </c>
       <c r="B207" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C207" t="s">
         <v>32</v>
@@ -6900,7 +6900,7 @@
         <v>341</v>
       </c>
       <c r="B208" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C208" t="s">
         <v>32</v>
@@ -6926,7 +6926,7 @@
         <v>341</v>
       </c>
       <c r="B209" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C209" t="s">
         <v>32</v>
@@ -6955,7 +6955,7 @@
         <v>341</v>
       </c>
       <c r="B210" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C210" t="s">
         <v>32</v>
@@ -6981,7 +6981,7 @@
         <v>341</v>
       </c>
       <c r="B211" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C211" t="s">
         <v>32</v>
@@ -7007,7 +7007,7 @@
         <v>341</v>
       </c>
       <c r="B212" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C212" t="s">
         <v>32</v>
@@ -7033,7 +7033,7 @@
         <v>341</v>
       </c>
       <c r="B213" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C213" t="s">
         <v>32</v>
@@ -7059,7 +7059,7 @@
         <v>341</v>
       </c>
       <c r="B214" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C214" t="s">
         <v>32</v>
@@ -7085,7 +7085,7 @@
         <v>341</v>
       </c>
       <c r="B215" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C215" t="s">
         <v>32</v>
@@ -7111,7 +7111,7 @@
         <v>341</v>
       </c>
       <c r="B216" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C216" t="s">
         <v>32</v>
@@ -7137,7 +7137,7 @@
         <v>341</v>
       </c>
       <c r="B217" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C217" t="s">
         <v>32</v>
@@ -7163,7 +7163,7 @@
         <v>341</v>
       </c>
       <c r="B218" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C218" t="s">
         <v>32</v>
@@ -7189,7 +7189,7 @@
         <v>341</v>
       </c>
       <c r="B219" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C219" t="s">
         <v>32</v>
@@ -7218,7 +7218,7 @@
         <v>341</v>
       </c>
       <c r="B220" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C220" t="s">
         <v>32</v>
@@ -7244,7 +7244,7 @@
         <v>341</v>
       </c>
       <c r="B221" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C221" t="s">
         <v>32</v>
@@ -7273,7 +7273,7 @@
         <v>341</v>
       </c>
       <c r="B222" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C222" t="s">
         <v>32</v>
@@ -7299,7 +7299,7 @@
         <v>341</v>
       </c>
       <c r="B223" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C223" t="s">
         <v>32</v>
@@ -7328,7 +7328,7 @@
         <v>341</v>
       </c>
       <c r="B224" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C224" t="s">
         <v>32</v>
@@ -7354,7 +7354,7 @@
         <v>341</v>
       </c>
       <c r="B225" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C225" t="s">
         <v>32</v>
@@ -7383,13 +7383,13 @@
         <v>341</v>
       </c>
       <c r="B226" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C226" t="s">
         <v>40</v>
       </c>
       <c r="D226" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E226" t="s">
         <v>335</v>
@@ -7409,13 +7409,13 @@
         <v>341</v>
       </c>
       <c r="B227" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C227" t="s">
         <v>40</v>
       </c>
       <c r="D227" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E227" t="s">
         <v>336</v>
@@ -7435,13 +7435,13 @@
         <v>341</v>
       </c>
       <c r="B228" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C228" t="s">
         <v>40</v>
       </c>
       <c r="D228" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E228" t="s">
         <v>337</v>
@@ -7461,13 +7461,13 @@
         <v>341</v>
       </c>
       <c r="B229" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C229" t="s">
         <v>40</v>
       </c>
       <c r="D229" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E229" t="s">
         <v>338</v>
@@ -7487,13 +7487,13 @@
         <v>341</v>
       </c>
       <c r="B230" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C230" t="s">
         <v>40</v>
       </c>
       <c r="D230" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E230" t="s">
         <v>335</v>
@@ -7513,13 +7513,13 @@
         <v>341</v>
       </c>
       <c r="B231" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C231" t="s">
         <v>40</v>
       </c>
       <c r="D231" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E231" t="s">
         <v>336</v>
@@ -7539,13 +7539,13 @@
         <v>341</v>
       </c>
       <c r="B232" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C232" t="s">
         <v>40</v>
       </c>
       <c r="D232" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E232" t="s">
         <v>337</v>
@@ -7565,13 +7565,13 @@
         <v>341</v>
       </c>
       <c r="B233" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C233" t="s">
         <v>40</v>
       </c>
       <c r="D233" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E233" t="s">
         <v>338</v>
@@ -7591,13 +7591,13 @@
         <v>341</v>
       </c>
       <c r="B234" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C234" t="s">
         <v>40</v>
       </c>
       <c r="D234" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E234" t="s">
         <v>335</v>
@@ -7614,13 +7614,13 @@
         <v>341</v>
       </c>
       <c r="B235" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C235" t="s">
         <v>40</v>
       </c>
       <c r="D235" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E235" t="s">
         <v>336</v>
@@ -7637,13 +7637,13 @@
         <v>341</v>
       </c>
       <c r="B236" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C236" t="s">
         <v>40</v>
       </c>
       <c r="D236" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E236" t="s">
         <v>337</v>
@@ -7660,13 +7660,13 @@
         <v>341</v>
       </c>
       <c r="B237" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C237" t="s">
         <v>40</v>
       </c>
       <c r="D237" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E237" t="s">
         <v>338</v>
@@ -7683,13 +7683,13 @@
         <v>341</v>
       </c>
       <c r="B238" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C238" t="s">
         <v>40</v>
       </c>
       <c r="D238" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E238" t="s">
         <v>335</v>
@@ -7706,13 +7706,13 @@
         <v>341</v>
       </c>
       <c r="B239" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C239" t="s">
         <v>40</v>
       </c>
       <c r="D239" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E239" t="s">
         <v>336</v>
@@ -7729,13 +7729,13 @@
         <v>341</v>
       </c>
       <c r="B240" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C240" t="s">
         <v>40</v>
       </c>
       <c r="D240" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E240" t="s">
         <v>337</v>
@@ -7752,13 +7752,13 @@
         <v>341</v>
       </c>
       <c r="B241" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C241" t="s">
         <v>40</v>
       </c>
       <c r="D241" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E241" t="s">
         <v>338</v>
@@ -7775,13 +7775,13 @@
         <v>341</v>
       </c>
       <c r="B242" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C242" t="s">
         <v>40</v>
       </c>
       <c r="D242" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E242" t="s">
         <v>335</v>
@@ -7798,13 +7798,13 @@
         <v>341</v>
       </c>
       <c r="B243" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C243" t="s">
         <v>40</v>
       </c>
       <c r="D243" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E243" t="s">
         <v>336</v>
@@ -7821,13 +7821,13 @@
         <v>341</v>
       </c>
       <c r="B244" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C244" t="s">
         <v>40</v>
       </c>
       <c r="D244" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E244" t="s">
         <v>337</v>
@@ -7844,13 +7844,13 @@
         <v>341</v>
       </c>
       <c r="B245" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C245" t="s">
         <v>40</v>
       </c>
       <c r="D245" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E245" t="s">
         <v>338</v>
@@ -7867,13 +7867,13 @@
         <v>341</v>
       </c>
       <c r="B246" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C246" t="s">
         <v>40</v>
       </c>
       <c r="D246" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E246" t="s">
         <v>335</v>
@@ -7890,13 +7890,13 @@
         <v>341</v>
       </c>
       <c r="B247" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C247" t="s">
         <v>40</v>
       </c>
       <c r="D247" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E247" t="s">
         <v>336</v>
@@ -7913,13 +7913,13 @@
         <v>341</v>
       </c>
       <c r="B248" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C248" t="s">
         <v>40</v>
       </c>
       <c r="D248" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E248" t="s">
         <v>337</v>
@@ -7936,13 +7936,13 @@
         <v>341</v>
       </c>
       <c r="B249" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C249" t="s">
         <v>40</v>
       </c>
       <c r="D249" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E249" t="s">
         <v>338</v>
@@ -7959,13 +7959,13 @@
         <v>341</v>
       </c>
       <c r="B250" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C250" t="s">
         <v>40</v>
       </c>
       <c r="D250" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E250" t="s">
         <v>335</v>
@@ -7982,13 +7982,13 @@
         <v>341</v>
       </c>
       <c r="B251" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C251" t="s">
         <v>40</v>
       </c>
       <c r="D251" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E251" t="s">
         <v>336</v>
@@ -8005,13 +8005,13 @@
         <v>341</v>
       </c>
       <c r="B252" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C252" t="s">
         <v>40</v>
       </c>
       <c r="D252" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E252" t="s">
         <v>337</v>
@@ -8028,13 +8028,13 @@
         <v>341</v>
       </c>
       <c r="B253" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C253" t="s">
         <v>40</v>
       </c>
       <c r="D253" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E253" t="s">
         <v>338</v>
@@ -8051,13 +8051,13 @@
         <v>341</v>
       </c>
       <c r="B254" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C254" t="s">
         <v>40</v>
       </c>
       <c r="D254" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E254" t="s">
         <v>335</v>
@@ -8074,13 +8074,13 @@
         <v>341</v>
       </c>
       <c r="B255" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C255" t="s">
         <v>40</v>
       </c>
       <c r="D255" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E255" t="s">
         <v>336</v>
@@ -8097,13 +8097,13 @@
         <v>341</v>
       </c>
       <c r="B256" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C256" t="s">
         <v>40</v>
       </c>
       <c r="D256" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E256" t="s">
         <v>337</v>
@@ -8120,13 +8120,13 @@
         <v>341</v>
       </c>
       <c r="B257" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C257" t="s">
         <v>40</v>
       </c>
       <c r="D257" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E257" t="s">
         <v>338</v>
@@ -8152,7 +8152,7 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8176,7 +8176,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -8202,7 +8202,7 @@
         <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -8228,7 +8228,7 @@
         <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -8254,7 +8254,7 @@
         <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -8280,7 +8280,7 @@
         <v>341</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -8306,7 +8306,7 @@
         <v>341</v>
       </c>
       <c r="B6" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8332,7 +8332,7 @@
         <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -8358,7 +8358,7 @@
         <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -8384,7 +8384,7 @@
         <v>341</v>
       </c>
       <c r="B9" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -8410,7 +8410,7 @@
         <v>341</v>
       </c>
       <c r="B10" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -8436,7 +8436,7 @@
         <v>341</v>
       </c>
       <c r="B11" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -8462,7 +8462,7 @@
         <v>341</v>
       </c>
       <c r="B12" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -8488,7 +8488,7 @@
         <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -8514,7 +8514,7 @@
         <v>341</v>
       </c>
       <c r="B14" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -8540,7 +8540,7 @@
         <v>341</v>
       </c>
       <c r="B15" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -8566,7 +8566,7 @@
         <v>341</v>
       </c>
       <c r="B16" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -8592,7 +8592,7 @@
         <v>341</v>
       </c>
       <c r="B17" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -8618,7 +8618,7 @@
         <v>341</v>
       </c>
       <c r="B18" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -8644,7 +8644,7 @@
         <v>341</v>
       </c>
       <c r="B19" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -8670,7 +8670,7 @@
         <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
@@ -8696,7 +8696,7 @@
         <v>341</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -8722,7 +8722,7 @@
         <v>341</v>
       </c>
       <c r="B22" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -8748,7 +8748,7 @@
         <v>341</v>
       </c>
       <c r="B23" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -8774,7 +8774,7 @@
         <v>341</v>
       </c>
       <c r="B24" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -8800,7 +8800,7 @@
         <v>341</v>
       </c>
       <c r="B25" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -8826,7 +8826,7 @@
         <v>341</v>
       </c>
       <c r="B26" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -8852,7 +8852,7 @@
         <v>341</v>
       </c>
       <c r="B27" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -8878,7 +8878,7 @@
         <v>341</v>
       </c>
       <c r="B28" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -8904,7 +8904,7 @@
         <v>341</v>
       </c>
       <c r="B29" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -8930,7 +8930,7 @@
         <v>341</v>
       </c>
       <c r="B30" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -8956,7 +8956,7 @@
         <v>341</v>
       </c>
       <c r="B31" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -8982,7 +8982,7 @@
         <v>341</v>
       </c>
       <c r="B32" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -9008,7 +9008,7 @@
         <v>341</v>
       </c>
       <c r="B33" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -9034,7 +9034,7 @@
         <v>341</v>
       </c>
       <c r="B34" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -9060,7 +9060,7 @@
         <v>341</v>
       </c>
       <c r="B35" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
@@ -9086,7 +9086,7 @@
         <v>341</v>
       </c>
       <c r="B36" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
@@ -9112,7 +9112,7 @@
         <v>341</v>
       </c>
       <c r="B37" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
@@ -9138,7 +9138,7 @@
         <v>341</v>
       </c>
       <c r="B38" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
@@ -9164,7 +9164,7 @@
         <v>341</v>
       </c>
       <c r="B39" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
@@ -9190,7 +9190,7 @@
         <v>341</v>
       </c>
       <c r="B40" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
@@ -9216,7 +9216,7 @@
         <v>341</v>
       </c>
       <c r="B41" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
@@ -9242,7 +9242,7 @@
         <v>341</v>
       </c>
       <c r="B42" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
@@ -9268,7 +9268,7 @@
         <v>341</v>
       </c>
       <c r="B43" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
@@ -9294,7 +9294,7 @@
         <v>341</v>
       </c>
       <c r="B44" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
@@ -9317,7 +9317,7 @@
         <v>341</v>
       </c>
       <c r="B45" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
@@ -9340,7 +9340,7 @@
         <v>341</v>
       </c>
       <c r="B46" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
@@ -9366,7 +9366,7 @@
         <v>341</v>
       </c>
       <c r="B47" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -9392,7 +9392,7 @@
         <v>341</v>
       </c>
       <c r="B48" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
@@ -9418,7 +9418,7 @@
         <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
@@ -9444,13 +9444,13 @@
         <v>341</v>
       </c>
       <c r="B50" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C50" t="s">
         <v>37</v>
       </c>
       <c r="D50" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E50" t="s">
         <v>333</v>
@@ -9470,13 +9470,13 @@
         <v>341</v>
       </c>
       <c r="B51" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C51" t="s">
         <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E51" t="s">
         <v>334</v>
@@ -9493,13 +9493,13 @@
         <v>341</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C52" t="s">
         <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E52" t="s">
         <v>333</v>
@@ -9519,13 +9519,13 @@
         <v>341</v>
       </c>
       <c r="B53" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C53" t="s">
         <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E53" t="s">
         <v>334</v>
@@ -9542,13 +9542,13 @@
         <v>341</v>
       </c>
       <c r="B54" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C54" t="s">
         <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E54" t="s">
         <v>333</v>
@@ -9565,13 +9565,13 @@
         <v>341</v>
       </c>
       <c r="B55" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C55" t="s">
         <v>37</v>
       </c>
       <c r="D55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E55" t="s">
         <v>334</v>
@@ -9588,13 +9588,13 @@
         <v>341</v>
       </c>
       <c r="B56" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C56" t="s">
         <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E56" t="s">
         <v>333</v>
@@ -9611,13 +9611,13 @@
         <v>341</v>
       </c>
       <c r="B57" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
       </c>
       <c r="D57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E57" t="s">
         <v>334</v>
@@ -9634,13 +9634,13 @@
         <v>341</v>
       </c>
       <c r="B58" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
       </c>
       <c r="D58" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E58" t="s">
         <v>333</v>
@@ -9657,13 +9657,13 @@
         <v>341</v>
       </c>
       <c r="B59" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C59" t="s">
         <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E59" t="s">
         <v>334</v>
@@ -9680,13 +9680,13 @@
         <v>341</v>
       </c>
       <c r="B60" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C60" t="s">
         <v>37</v>
       </c>
       <c r="D60" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E60" t="s">
         <v>333</v>
@@ -9703,13 +9703,13 @@
         <v>341</v>
       </c>
       <c r="B61" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C61" t="s">
         <v>37</v>
       </c>
       <c r="D61" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E61" t="s">
         <v>334</v>
@@ -9726,13 +9726,13 @@
         <v>341</v>
       </c>
       <c r="B62" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C62" t="s">
         <v>37</v>
       </c>
       <c r="D62" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E62" t="s">
         <v>333</v>
@@ -9749,13 +9749,13 @@
         <v>341</v>
       </c>
       <c r="B63" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C63" t="s">
         <v>37</v>
       </c>
       <c r="D63" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E63" t="s">
         <v>334</v>
@@ -9772,13 +9772,13 @@
         <v>341</v>
       </c>
       <c r="B64" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C64" t="s">
         <v>37</v>
       </c>
       <c r="D64" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E64" t="s">
         <v>333</v>
@@ -9795,13 +9795,13 @@
         <v>341</v>
       </c>
       <c r="B65" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C65" t="s">
         <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E65" t="s">
         <v>334</v>
@@ -9818,7 +9818,7 @@
         <v>341</v>
       </c>
       <c r="B66" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C66" t="s">
         <v>18</v>
@@ -9844,7 +9844,7 @@
         <v>341</v>
       </c>
       <c r="B67" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C67" t="s">
         <v>18</v>
@@ -9870,7 +9870,7 @@
         <v>341</v>
       </c>
       <c r="B68" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C68" t="s">
         <v>18</v>
@@ -9896,7 +9896,7 @@
         <v>341</v>
       </c>
       <c r="B69" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C69" t="s">
         <v>18</v>
@@ -9922,7 +9922,7 @@
         <v>341</v>
       </c>
       <c r="B70" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C70" t="s">
         <v>18</v>
@@ -9948,7 +9948,7 @@
         <v>341</v>
       </c>
       <c r="B71" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
@@ -9974,7 +9974,7 @@
         <v>341</v>
       </c>
       <c r="B72" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C72" t="s">
         <v>18</v>
@@ -10000,7 +10000,7 @@
         <v>341</v>
       </c>
       <c r="B73" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C73" t="s">
         <v>18</v>
@@ -10026,7 +10026,7 @@
         <v>341</v>
       </c>
       <c r="B74" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C74" t="s">
         <v>18</v>
@@ -10052,7 +10052,7 @@
         <v>341</v>
       </c>
       <c r="B75" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C75" t="s">
         <v>18</v>
@@ -10078,7 +10078,7 @@
         <v>341</v>
       </c>
       <c r="B76" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C76" t="s">
         <v>18</v>
@@ -10104,7 +10104,7 @@
         <v>341</v>
       </c>
       <c r="B77" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C77" t="s">
         <v>18</v>
@@ -10130,7 +10130,7 @@
         <v>341</v>
       </c>
       <c r="B78" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C78" t="s">
         <v>18</v>
@@ -10156,7 +10156,7 @@
         <v>341</v>
       </c>
       <c r="B79" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C79" t="s">
         <v>18</v>
@@ -10182,7 +10182,7 @@
         <v>341</v>
       </c>
       <c r="B80" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C80" t="s">
         <v>18</v>
@@ -10208,7 +10208,7 @@
         <v>341</v>
       </c>
       <c r="B81" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C81" t="s">
         <v>18</v>
@@ -10234,7 +10234,7 @@
         <v>341</v>
       </c>
       <c r="B82" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C82" t="s">
         <v>28</v>
@@ -10260,7 +10260,7 @@
         <v>341</v>
       </c>
       <c r="B83" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
@@ -10286,7 +10286,7 @@
         <v>341</v>
       </c>
       <c r="B84" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
@@ -10312,7 +10312,7 @@
         <v>341</v>
       </c>
       <c r="B85" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C85" t="s">
         <v>28</v>
@@ -10338,7 +10338,7 @@
         <v>341</v>
       </c>
       <c r="B86" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C86" t="s">
         <v>28</v>
@@ -10364,7 +10364,7 @@
         <v>341</v>
       </c>
       <c r="B87" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C87" t="s">
         <v>28</v>
@@ -10390,7 +10390,7 @@
         <v>341</v>
       </c>
       <c r="B88" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C88" t="s">
         <v>28</v>
@@ -10416,7 +10416,7 @@
         <v>341</v>
       </c>
       <c r="B89" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C89" t="s">
         <v>28</v>
@@ -10442,7 +10442,7 @@
         <v>341</v>
       </c>
       <c r="B90" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -10468,7 +10468,7 @@
         <v>341</v>
       </c>
       <c r="B91" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
@@ -10494,7 +10494,7 @@
         <v>341</v>
       </c>
       <c r="B92" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C92" t="s">
         <v>28</v>
@@ -10520,7 +10520,7 @@
         <v>341</v>
       </c>
       <c r="B93" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C93" t="s">
         <v>28</v>
@@ -10546,7 +10546,7 @@
         <v>341</v>
       </c>
       <c r="B94" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C94" t="s">
         <v>28</v>
@@ -10572,7 +10572,7 @@
         <v>341</v>
       </c>
       <c r="B95" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C95" t="s">
         <v>28</v>
@@ -10598,7 +10598,7 @@
         <v>341</v>
       </c>
       <c r="B96" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C96" t="s">
         <v>28</v>
@@ -10624,7 +10624,7 @@
         <v>341</v>
       </c>
       <c r="B97" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -10650,7 +10650,7 @@
         <v>341</v>
       </c>
       <c r="B98" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C98" t="s">
         <v>32</v>
@@ -10676,7 +10676,7 @@
         <v>341</v>
       </c>
       <c r="B99" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C99" t="s">
         <v>32</v>
@@ -10702,7 +10702,7 @@
         <v>341</v>
       </c>
       <c r="B100" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C100" t="s">
         <v>32</v>
@@ -10728,7 +10728,7 @@
         <v>341</v>
       </c>
       <c r="B101" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C101" t="s">
         <v>32</v>
@@ -10754,7 +10754,7 @@
         <v>341</v>
       </c>
       <c r="B102" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C102" t="s">
         <v>32</v>
@@ -10780,7 +10780,7 @@
         <v>341</v>
       </c>
       <c r="B103" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C103" t="s">
         <v>32</v>
@@ -10806,7 +10806,7 @@
         <v>341</v>
       </c>
       <c r="B104" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C104" t="s">
         <v>32</v>
@@ -10832,7 +10832,7 @@
         <v>341</v>
       </c>
       <c r="B105" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C105" t="s">
         <v>32</v>
@@ -10858,7 +10858,7 @@
         <v>341</v>
       </c>
       <c r="B106" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C106" t="s">
         <v>32</v>
@@ -10884,7 +10884,7 @@
         <v>341</v>
       </c>
       <c r="B107" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C107" t="s">
         <v>32</v>
@@ -10910,7 +10910,7 @@
         <v>341</v>
       </c>
       <c r="B108" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C108" t="s">
         <v>32</v>
@@ -10936,7 +10936,7 @@
         <v>341</v>
       </c>
       <c r="B109" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C109" t="s">
         <v>32</v>
@@ -10962,7 +10962,7 @@
         <v>341</v>
       </c>
       <c r="B110" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C110" t="s">
         <v>32</v>
@@ -10988,7 +10988,7 @@
         <v>341</v>
       </c>
       <c r="B111" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C111" t="s">
         <v>32</v>
@@ -11014,7 +11014,7 @@
         <v>341</v>
       </c>
       <c r="B112" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C112" t="s">
         <v>32</v>
@@ -11040,7 +11040,7 @@
         <v>341</v>
       </c>
       <c r="B113" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C113" t="s">
         <v>32</v>
@@ -11066,13 +11066,13 @@
         <v>341</v>
       </c>
       <c r="B114" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C114" t="s">
         <v>40</v>
       </c>
       <c r="D114" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E114" t="s">
         <v>333</v>
@@ -11092,13 +11092,13 @@
         <v>341</v>
       </c>
       <c r="B115" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C115" t="s">
         <v>40</v>
       </c>
       <c r="D115" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E115" t="s">
         <v>334</v>
@@ -11115,13 +11115,13 @@
         <v>341</v>
       </c>
       <c r="B116" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C116" t="s">
         <v>40</v>
       </c>
       <c r="D116" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E116" t="s">
         <v>333</v>
@@ -11141,13 +11141,13 @@
         <v>341</v>
       </c>
       <c r="B117" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C117" t="s">
         <v>40</v>
       </c>
       <c r="D117" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E117" t="s">
         <v>334</v>
@@ -11164,13 +11164,13 @@
         <v>341</v>
       </c>
       <c r="B118" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C118" t="s">
         <v>40</v>
       </c>
       <c r="D118" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E118" t="s">
         <v>333</v>
@@ -11187,13 +11187,13 @@
         <v>341</v>
       </c>
       <c r="B119" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C119" t="s">
         <v>40</v>
       </c>
       <c r="D119" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E119" t="s">
         <v>334</v>
@@ -11210,13 +11210,13 @@
         <v>341</v>
       </c>
       <c r="B120" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C120" t="s">
         <v>40</v>
       </c>
       <c r="D120" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E120" t="s">
         <v>333</v>
@@ -11233,13 +11233,13 @@
         <v>341</v>
       </c>
       <c r="B121" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C121" t="s">
         <v>40</v>
       </c>
       <c r="D121" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E121" t="s">
         <v>334</v>
@@ -11256,13 +11256,13 @@
         <v>341</v>
       </c>
       <c r="B122" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C122" t="s">
         <v>40</v>
       </c>
       <c r="D122" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E122" t="s">
         <v>333</v>
@@ -11279,13 +11279,13 @@
         <v>341</v>
       </c>
       <c r="B123" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C123" t="s">
         <v>40</v>
       </c>
       <c r="D123" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E123" t="s">
         <v>334</v>
@@ -11302,13 +11302,13 @@
         <v>341</v>
       </c>
       <c r="B124" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C124" t="s">
         <v>40</v>
       </c>
       <c r="D124" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E124" t="s">
         <v>333</v>
@@ -11325,13 +11325,13 @@
         <v>341</v>
       </c>
       <c r="B125" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C125" t="s">
         <v>40</v>
       </c>
       <c r="D125" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E125" t="s">
         <v>334</v>
@@ -11348,13 +11348,13 @@
         <v>341</v>
       </c>
       <c r="B126" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C126" t="s">
         <v>40</v>
       </c>
       <c r="D126" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E126" t="s">
         <v>333</v>
@@ -11371,13 +11371,13 @@
         <v>341</v>
       </c>
       <c r="B127" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C127" t="s">
         <v>40</v>
       </c>
       <c r="D127" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E127" t="s">
         <v>334</v>
@@ -11394,13 +11394,13 @@
         <v>341</v>
       </c>
       <c r="B128" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C128" t="s">
         <v>40</v>
       </c>
       <c r="D128" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E128" t="s">
         <v>333</v>
@@ -11417,13 +11417,13 @@
         <v>341</v>
       </c>
       <c r="B129" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C129" t="s">
         <v>40</v>
       </c>
       <c r="D129" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E129" t="s">
         <v>334</v>
@@ -11444,21 +11444,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDA4FEBE11D32545B6C4D443ADFB229A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa29c2c3225ad03fb09b8df90fa91a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b103a3be-6c61-44b0-93c5-2b779aa38a01" xmlns:ns3="56612388-9f28-4625-93a0-6879c02082d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c16c82533632c11d7fcceef7f9e9ea5" ns2:_="" ns3:_="">
     <xsd:import namespace="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
@@ -11623,32 +11608,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
-    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CADB2AF-8FF4-4CD3-86AB-7AA08F493F37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11665,4 +11640,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
+    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>